<commit_message>
Added requirements and design documents
</commit_message>
<xml_diff>
--- a/project_docs/timekeeping.xlsx
+++ b/project_docs/timekeeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KSU\CIS598\CIS598-project\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92D9D08-02FD-41CE-A78E-B4671EDA9750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFA6899-B5C9-4EC8-A58E-C48AE5B9AFE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>design presentation</t>
+  </si>
+  <si>
+    <t>writing requirements/design documents</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC34BB06-34CF-439A-B249-848A3D105895}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f>C2-B2-TIME(0,D2,0)</f>
+        <f t="shared" ref="E2:E8" si="0">C2-B2-TIME(0,D2,0)</f>
         <v>3.1944444444444553E-2</v>
       </c>
       <c r="F2" t="s">
@@ -484,7 +487,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <f>C3-B3-TIME(0,D3,0)</f>
+        <f t="shared" si="0"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F3" t="s">
@@ -505,7 +508,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2">
-        <f>C4-B4-TIME(0,D4,0)</f>
+        <f t="shared" si="0"/>
         <v>7.9166666666666566E-2</v>
       </c>
       <c r="F4" t="s">
@@ -526,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f>C5-B5-TIME(0,D5,0)</f>
+        <f t="shared" si="0"/>
         <v>3.4027777777777768E-2</v>
       </c>
       <c r="F5" t="s">
@@ -547,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f>C6-B6-TIME(0,D6,0)</f>
+        <f t="shared" si="0"/>
         <v>9.3055555555555503E-2</v>
       </c>
       <c r="F6" t="s">
@@ -568,11 +571,32 @@
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <f>C7-B7-TIME(0,D7,0)</f>
+        <f t="shared" si="0"/>
         <v>6.5277777777777879E-2</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44146</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.65902777777777777</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.74722222222222223</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>8.1250000000000017E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added parsing for assembly, solve, and summarize
</commit_message>
<xml_diff>
--- a/project_docs/timekeeping.xlsx
+++ b/project_docs/timekeeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KSU\CIS598\CIS598-project\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFA6899-B5C9-4EC8-A58E-C48AE5B9AFE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1D5496-03D9-4321-AA9F-FCAA0F2E6970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -69,8 +69,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,10 +106,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,39 +425,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC34BB06-34CF-439A-B249-848A3D105895}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -466,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E8" si="0">C2-B2-TIME(0,D2,0)</f>
+        <f t="shared" ref="E2:E9" si="0">C2-B2-TIME(0,D2,0)</f>
         <v>3.1944444444444553E-2</v>
       </c>
       <c r="F2" t="s">
@@ -599,7 +609,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44147</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.61041666666666672</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2361111111111065E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wrote evaluate() function to solve expressions
</commit_message>
<xml_diff>
--- a/project_docs/timekeeping.xlsx
+++ b/project_docs/timekeeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KSU\CIS598\CIS598-project\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1D5496-03D9-4321-AA9F-FCAA0F2E6970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FFE2EB-905A-4319-BD52-525DD444C157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC34BB06-34CF-439A-B249-848A3D105895}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E9" si="0">C2-B2-TIME(0,D2,0)</f>
+        <f t="shared" ref="E2:E11" si="0">C2-B2-TIME(0,D2,0)</f>
         <v>3.1944444444444553E-2</v>
       </c>
       <c r="F2" t="s">
@@ -627,6 +627,48 @@
         <v>4.2361111111111065E-2</v>
       </c>
       <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44149</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1527777777777857E-2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44150</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.5805555555555556</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.60902777777777783</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8472222222222232E-2</v>
+      </c>
+      <c r="F11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ParseTreeExpressionSubtract and cleaned up Main.go
</commit_message>
<xml_diff>
--- a/project_docs/timekeeping.xlsx
+++ b/project_docs/timekeeping.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KSU\CIS598\CIS598-project\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FFE2EB-905A-4319-BD52-525DD444C157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9874AD5-5B9D-4B19-912D-021B118FFFDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -106,11 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC34BB06-34CF-439A-B249-848A3D105895}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G16" sqref="G16:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +478,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E11" si="0">C2-B2-TIME(0,D2,0)</f>
+        <f t="shared" ref="E2:E15" si="0">C2-B2-TIME(0,D2,0)</f>
         <v>3.1944444444444553E-2</v>
       </c>
       <c r="F2" t="s">
@@ -671,6 +673,99 @@
       <c r="F11" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>7.8472222222222276E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>9.6527777777777671E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>8.6111111111111138E-2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.76944444444444438</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9444444444444486E-2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Codebase is code complete
</commit_message>
<xml_diff>
--- a/project_docs/timekeeping.xlsx
+++ b/project_docs/timekeeping.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KSU\CIS598\CIS598-project\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9874AD5-5B9D-4B19-912D-021B118FFFDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E32DFA8-2D39-4DDC-9AE3-ED0630FC1E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +63,15 @@
   </si>
   <si>
     <t>writing requirements/design documents</t>
+  </si>
+  <si>
+    <t>creating final presentation</t>
+  </si>
+  <si>
+    <t>editing final presentation</t>
+  </si>
+  <si>
+    <t>editing final presentation; preparing demo</t>
   </si>
 </sst>
 </file>
@@ -430,14 +438,14 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:H21"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
     <col min="7" max="7" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -478,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E15" si="0">C2-B2-TIME(0,D2,0)</f>
+        <f t="shared" ref="E2:E18" si="0">C2-B2-TIME(0,D2,0)</f>
         <v>3.1944444444444553E-2</v>
       </c>
       <c r="F2" t="s">
@@ -758,13 +766,74 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44170</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.62986111111111109</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2916666666666696E-2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44172</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.69513888888888886</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8888888888888862E-2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G20" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created UML diagrams and final report
</commit_message>
<xml_diff>
--- a/project_docs/timekeeping.xlsx
+++ b/project_docs/timekeeping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KSU\CIS598\CIS598-project\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E32DFA8-2D39-4DDC-9AE3-ED0630FC1E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABEDD79-0BC1-49B7-8395-C701449C70FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{DDE4787D-2D9A-485C-85C7-8A7B5D65DB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>editing final presentation; preparing demo</t>
+  </si>
+  <si>
+    <t>creating final UML diagrams and report</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E18" si="0">C2-B2-TIME(0,D2,0)</f>
+        <f t="shared" ref="E2:E19" si="0">C2-B2-TIME(0,D2,0)</f>
         <v>3.1944444444444553E-2</v>
       </c>
       <c r="F2" t="s">
@@ -831,6 +834,25 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3055555555555558E-2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>